<commit_message>
Add plotting functions to CrossSection class
</commit_message>
<xml_diff>
--- a/XC-template1.xlsx
+++ b/XC-template1.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr backupFile="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="11295" windowHeight="6750"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="11295" windowHeight="6750" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="xc1" sheetId="1" r:id="rId1"/>
+    <sheet name="xc2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
   <si>
     <t>FIELDS Template</t>
   </si>
@@ -106,22 +107,40 @@
     <t>Input Value</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
     <t>Voltage (kV)</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>2a</t>
+  </si>
+  <si>
+    <t>2b</t>
+  </si>
+  <si>
+    <t>2c</t>
+  </si>
+  <si>
+    <t>xc1</t>
+  </si>
+  <si>
+    <t>test cross section</t>
+  </si>
+  <si>
+    <t>1g</t>
+  </si>
+  <si>
+    <t>xc2</t>
+  </si>
+  <si>
+    <t>2g</t>
   </si>
 </sst>
 </file>
@@ -576,7 +595,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>test</c:v>
+              <c:v>xc1</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -612,9 +631,18 @@
                   <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
@@ -627,13 +655,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -661,7 +698,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -673,7 +713,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -720,7 +763,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>18.900000000000002</c:v>
+                  <c:v>33.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -768,7 +811,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>18.900000000000002</c:v>
+                  <c:v>33.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -777,23 +820,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="85395712"/>
-        <c:axId val="100534912"/>
+        <c:axId val="81744640"/>
+        <c:axId val="81746176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85395712"/>
+        <c:axId val="81744640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100534912"/>
+        <c:crossAx val="81746176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="100534912"/>
+        <c:axId val="81746176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -801,7 +844,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85395712"/>
+        <c:crossAx val="81744640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -814,13 +857,327 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>'xc2'!$B$5</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>xc2</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Conductor Coordinates</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc2'!$D$5:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc2'!$E$5:$E$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ground Wire Coordinates</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc2'!$M$5:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc2'!$N$5:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Right ROW Edge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc2'!$S$7:$S$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc2'!$R$5:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>36.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Left ROW Edge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc2'!$S$5:$S$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc2'!$R$5:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>36.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="83155968"/>
+        <c:axId val="83297024"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="83155968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="83297024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="83297024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="83155968"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1142,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1256,7 +1613,7 @@
         <v>24</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>15</v>
@@ -1294,7 +1651,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>31</v>
@@ -1303,7 +1660,7 @@
         <v>-10</v>
       </c>
       <c r="E5" s="9">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="F5" s="9">
         <v>1</v>
@@ -1325,13 +1682,13 @@
         <v>0</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="M5" s="9">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="N5" s="9">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="O5" s="9">
         <v>1</v>
@@ -1344,7 +1701,7 @@
       </c>
       <c r="R5" s="28">
         <f>MAX(E5:E25,N5:N25)*1.05</f>
-        <v>18.900000000000002</v>
+        <v>33.6</v>
       </c>
       <c r="S5" s="28">
         <f>B12</f>
@@ -1356,16 +1713,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>32</v>
       </c>
       <c r="D6" s="9">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="E6" s="9">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F6" s="9">
         <v>1</v>
@@ -1385,7 +1742,24 @@
       <c r="K6" s="14">
         <v>120</v>
       </c>
-      <c r="L6" s="9"/>
+      <c r="L6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="9">
+        <v>10</v>
+      </c>
+      <c r="N6" s="9">
+        <v>32</v>
+      </c>
+      <c r="O6" s="9">
+        <v>1</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>0</v>
+      </c>
       <c r="R6" s="28">
         <v>0</v>
       </c>
@@ -1405,10 +1779,10 @@
         <v>33</v>
       </c>
       <c r="D7" s="8">
-        <v>10</v>
+        <v>-5</v>
       </c>
       <c r="E7" s="8">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F7" s="8">
         <v>1</v>
@@ -1442,6 +1816,33 @@
       <c r="B8" s="18">
         <v>100</v>
       </c>
+      <c r="C8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="9">
+        <v>5</v>
+      </c>
+      <c r="E8" s="9">
+        <v>25</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>500</v>
+      </c>
+      <c r="J8" s="9">
+        <v>100</v>
+      </c>
+      <c r="K8" s="14">
+        <v>0</v>
+      </c>
       <c r="L8" s="9"/>
       <c r="R8" s="28"/>
       <c r="S8" s="28">
@@ -1454,7 +1855,34 @@
         <v>25</v>
       </c>
       <c r="B9" s="17">
-        <v>25</v>
+        <v>50</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="9">
+        <v>10</v>
+      </c>
+      <c r="E9" s="9">
+        <v>22</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>500</v>
+      </c>
+      <c r="J9" s="9">
+        <v>100</v>
+      </c>
+      <c r="K9" s="14">
+        <v>120</v>
       </c>
       <c r="L9" s="9"/>
     </row>
@@ -1465,15 +1893,33 @@
       <c r="B10" s="17">
         <v>1</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="15"/>
+      <c r="C10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="8">
+        <v>10</v>
+      </c>
+      <c r="E10" s="8">
+        <v>28</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
+        <v>500</v>
+      </c>
+      <c r="J10" s="8">
+        <v>100</v>
+      </c>
+      <c r="K10" s="15">
+        <v>240</v>
+      </c>
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:19">
@@ -1596,4 +2042,552 @@
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.5703125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.5703125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="25" customFormat="1" ht="15">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:19" s="26" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75">
+      <c r="A3" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="33"/>
+    </row>
+    <row r="4" spans="1:19" ht="38.25">
+      <c r="A4" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="9">
+        <v>-5</v>
+      </c>
+      <c r="E5" s="9">
+        <v>23</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9">
+        <f>F5*G5</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>500</v>
+      </c>
+      <c r="J5" s="9">
+        <v>100</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="9">
+        <v>-2</v>
+      </c>
+      <c r="N5" s="9">
+        <v>35</v>
+      </c>
+      <c r="O5" s="9">
+        <v>1</v>
+      </c>
+      <c r="P5" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>0</v>
+      </c>
+      <c r="R5" s="28">
+        <f>MAX(E5:E25,N5:N25)*1.05</f>
+        <v>36.75</v>
+      </c>
+      <c r="S5" s="28">
+        <f>B12</f>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="9">
+        <v>-7</v>
+      </c>
+      <c r="E6" s="9">
+        <v>27</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <v>500</v>
+      </c>
+      <c r="J6" s="9">
+        <v>100</v>
+      </c>
+      <c r="K6" s="14">
+        <v>120</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="M6" s="9">
+        <v>2</v>
+      </c>
+      <c r="N6" s="9">
+        <v>35</v>
+      </c>
+      <c r="O6" s="9">
+        <v>1</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>0</v>
+      </c>
+      <c r="R6" s="28">
+        <v>0</v>
+      </c>
+      <c r="S6" s="28">
+        <f>B12</f>
+        <v>-25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18">
+        <v>60</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="8">
+        <v>-5</v>
+      </c>
+      <c r="E7" s="8">
+        <v>32</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
+        <v>500</v>
+      </c>
+      <c r="J7" s="8">
+        <v>100</v>
+      </c>
+      <c r="K7" s="15">
+        <v>240</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28">
+        <f>B13</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="18">
+        <v>100</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="9">
+        <v>5</v>
+      </c>
+      <c r="E8" s="9">
+        <v>32</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>500</v>
+      </c>
+      <c r="J8" s="9">
+        <v>100</v>
+      </c>
+      <c r="K8" s="14">
+        <v>0</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28">
+        <f>B13</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="17">
+        <v>50</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="9">
+        <v>7</v>
+      </c>
+      <c r="E9" s="9">
+        <v>27</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>500</v>
+      </c>
+      <c r="J9" s="9">
+        <v>100</v>
+      </c>
+      <c r="K9" s="14">
+        <v>120</v>
+      </c>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="17">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="8">
+        <v>5</v>
+      </c>
+      <c r="E10" s="8">
+        <v>23</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
+        <v>500</v>
+      </c>
+      <c r="J10" s="8">
+        <v>100</v>
+      </c>
+      <c r="K10" s="15">
+        <v>240</v>
+      </c>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="18">
+        <v>3</v>
+      </c>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="17">
+        <v>-25</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:19" ht="13.5" thickBot="1">
+      <c r="A13" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="20">
+        <v>25</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:19" ht="12.75" customHeight="1">
+      <c r="A14" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="C16" s="12"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="3:12">
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="3:12">
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="3:12">
+      <c r="C19" s="12"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="22" spans="3:12">
+      <c r="C22" s="12"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="25" spans="3:12">
+      <c r="C25" s="12"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="A14:B15"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="0.75" header="0.5" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;L&amp;"-,Regular"&amp;9Draft&amp;C&amp;"Times New Roman,Bold"&amp;11 </oddHeader>
+    <oddFooter>&amp;L&amp;K4D4D4DG&amp;8RADIENT&amp;"Cambria,Regular"&amp;6
+&amp;"-,Regular"&amp;K4D4D4D
+&amp;Z&amp;F\&amp;A&amp;R&amp;"-,Regular"&amp;9Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>